<commit_message>
Mostly updated branch data results committed
</commit_message>
<xml_diff>
--- a/Microgrgrid2k15/MicrogridVersion1/RunPVControlsModular/PVControllers.xlsx
+++ b/Microgrgrid2k15/MicrogridVersion1/RunPVControlsModular/PVControllers.xlsx
@@ -683,27 +683,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9279,7 +9259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -10726,7 +10706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA94"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A50" workbookViewId="0">
       <selection activeCell="AA76" sqref="AA76"/>
     </sheetView>
   </sheetViews>

</xml_diff>